<commit_message>
Added United Express tracking support
</commit_message>
<xml_diff>
--- a/FEDEX/split_datasets/UNITED_EXPRESS.xlsx
+++ b/FEDEX/split_datasets/UNITED_EXPRESS.xlsx
@@ -562,7 +562,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Delivered</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
@@ -620,7 +620,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Delivered</t>
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
@@ -680,7 +680,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Delivered</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Delivered</t>
         </is>
       </c>
       <c r="N5" t="inlineStr"/>

</xml_diff>